<commit_message>
refactoring dca analysis into class structure
</commit_message>
<xml_diff>
--- a/tests/resources/test_master_4_2018_dcas.xlsx
+++ b/tests/resources/test_master_4_2018_dcas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="74">
   <si>
     <t xml:space="preserve">Project/Programme Name</t>
   </si>
@@ -240,6 +240,9 @@
   </si>
   <si>
     <t xml:space="preserve">Re-baseline this quarter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Forecast</t>
   </si>
 </sst>
 </file>
@@ -249,7 +252,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -306,12 +309,6 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -389,7 +386,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -473,11 +470,11 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="59" zoomScaleNormal="59" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A36" activeCellId="0" sqref="A36"/>
+      <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="C35" activeCellId="0" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -931,6 +928,26 @@
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="8" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>672</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>268</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>6427</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <v>738</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>516</v>
       </c>
     </row>
     <row r="1046595" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>